<commit_message>
backing up my laptop
</commit_message>
<xml_diff>
--- a/exp/gromacs_sse4.1/bin/tx_analysis.xlsx
+++ b/exp/gromacs_sse4.1/bin/tx_analysis.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="58">
   <si>
     <t xml:space="preserve">Actual Tx</t>
   </si>
@@ -100,6 +100,15 @@
     <t xml:space="preserve">Cycles</t>
   </si>
   <si>
+    <t xml:space="preserve">OSG (22%  adj)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tx_base_prederr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tx_max_prederr</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not OSG, Tx from Predicted number of cycles</t>
   </si>
   <si>
@@ -151,7 +160,22 @@
     <t xml:space="preserve">% Pred. Error (100000)</t>
   </si>
   <si>
+    <t xml:space="preserve">Cycles Prederr, Tx Prederr with actual clockspeed comparison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tx Prediction Error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Percent Diff</t>
+  </si>
+  <si>
     <t xml:space="preserve">Not OSG, Tx from Predicted number of cycles, adjusted for instruction rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(pred_tx – actual_tx) / actual_tx</t>
   </si>
   <si>
     <t xml:space="preserve">OSG, Tx from Predicted number of cycles, partial data</t>
@@ -252,7 +276,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -277,8 +301,16 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -306,24 +338,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W150"/>
+  <dimension ref="A1:AE150"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B85" activeCellId="0" sqref="B85"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J106" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O106" activeCellId="0" sqref="O106:T114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="16.7142857142857"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.90816326530612"/>
-    <col collapsed="false" hidden="false" max="14" min="6" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -832,6 +863,15 @@
       <c r="I15" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="J15" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="M15" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="N15" s="0" t="s">
+        <v>28</v>
+      </c>
       <c r="P15" s="4" t="n">
         <v>3419569391804.87</v>
       </c>
@@ -874,6 +914,24 @@
       <c r="I16" s="2" t="n">
         <v>310453426772</v>
       </c>
+      <c r="J16" s="0" t="n">
+        <f aca="false">I16*1.24</f>
+        <v>384962249197.28</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>153.984899678912</v>
+      </c>
+      <c r="L16" s="0" t="n">
+        <v>122.573844874382</v>
+      </c>
+      <c r="M16" s="0" t="n">
+        <f aca="false">100*ABS(K16-E4)/E4</f>
+        <v>42.446563764388</v>
+      </c>
+      <c r="N16" s="6" t="n">
+        <f aca="false">100*ABS(E4-L16)/E4</f>
+        <v>13.3891897592085</v>
+      </c>
       <c r="O16" s="4"/>
       <c r="P16" s="4" t="n">
         <v>6858000854399.23</v>
@@ -917,6 +975,24 @@
       <c r="I17" s="2" t="n">
         <v>1546280435401</v>
       </c>
+      <c r="J17" s="0" t="n">
+        <f aca="false">I17*1.24</f>
+        <v>1917387739897.24</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>766.955095958896</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>610.505544074181</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <f aca="false">100*ABS(K17-E5)/E5</f>
+        <v>42.9838265143723</v>
+      </c>
+      <c r="N17" s="6" t="n">
+        <f aca="false">100*ABS(E5-L17)/E5</f>
+        <v>13.8168574143532</v>
+      </c>
       <c r="O17" s="4"/>
       <c r="P17" s="4" t="n">
         <v>10293760899846.7</v>
@@ -947,6 +1023,24 @@
       <c r="I18" s="2" t="n">
         <v>3090814069269</v>
       </c>
+      <c r="J18" s="0" t="n">
+        <f aca="false">I18*1.24</f>
+        <v>3832609445893.56</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>1533.04377835742</v>
+      </c>
+      <c r="L18" s="0" t="n">
+        <v>1220.32141246219</v>
+      </c>
+      <c r="M18" s="0" t="n">
+        <f aca="false">100*ABS(K18-E6)/E6</f>
+        <v>42.5343047673936</v>
+      </c>
+      <c r="N18" s="6" t="n">
+        <f aca="false">100*ABS(E6-L18)/E6</f>
+        <v>13.459032660129</v>
+      </c>
       <c r="O18" s="4"/>
       <c r="P18" s="4" t="n">
         <v>13730792068590.5</v>
@@ -990,6 +1084,24 @@
       <c r="I19" s="2" t="n">
         <v>7726299241085</v>
       </c>
+      <c r="J19" s="0" t="n">
+        <f aca="false">I19*1.24</f>
+        <v>9580611058945.4</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>3832.24442357816</v>
+      </c>
+      <c r="L19" s="0" t="n">
+        <v>3050.51296897207</v>
+      </c>
+      <c r="M19" s="0" t="n">
+        <f aca="false">100*ABS(K19-E7)/E7</f>
+        <v>45.7980343060699</v>
+      </c>
+      <c r="N19" s="6" t="n">
+        <f aca="false">100*ABS(E7-L19)/E7</f>
+        <v>16.0570008961043</v>
+      </c>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
       <c r="Q19" s="3"/>
@@ -1014,6 +1126,24 @@
       <c r="I20" s="2" t="n">
         <v>15454218942566</v>
       </c>
+      <c r="J20" s="0" t="n">
+        <f aca="false">I20*1.24</f>
+        <v>19163231488781.8</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>7665.29259551274</v>
+      </c>
+      <c r="L20" s="0" t="n">
+        <v>6101.6657313691</v>
+      </c>
+      <c r="M20" s="0" t="n">
+        <f aca="false">100*ABS(K20-E8)/E8</f>
+        <v>44.0025814164008</v>
+      </c>
+      <c r="N20" s="6" t="n">
+        <f aca="false">100*ABS(E8-L20)/E8</f>
+        <v>14.62779865331</v>
+      </c>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
       <c r="Q20" s="3"/>
@@ -1025,6 +1155,24 @@
       <c r="I21" s="2" t="n">
         <v>23176329755349</v>
       </c>
+      <c r="J21" s="0" t="n">
+        <f aca="false">I21*1.24</f>
+        <v>28738648896632.8</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>11495.4595586531</v>
+      </c>
+      <c r="L21" s="0" t="n">
+        <v>9150.52501667501</v>
+      </c>
+      <c r="M21" s="0" t="n">
+        <f aca="false">100*ABS(K21-E9)/E9</f>
+        <v>43.0319698271509</v>
+      </c>
+      <c r="N21" s="6" t="n">
+        <f aca="false">100*ABS(E9-L21)/E9</f>
+        <v>13.8551800743319</v>
+      </c>
       <c r="O21" s="4"/>
       <c r="P21" s="0" t="s">
         <v>6</v>
@@ -1038,7 +1186,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1050,6 +1198,24 @@
       <c r="I22" s="2" t="n">
         <v>30905562822446</v>
       </c>
+      <c r="J22" s="0" t="n">
+        <f aca="false">I22*1.24</f>
+        <v>38322897899833</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>15329.1591599332</v>
+      </c>
+      <c r="L22" s="0" t="n">
+        <v>12202.1963247198</v>
+      </c>
+      <c r="M22" s="0" t="n">
+        <f aca="false">100*ABS(K22-E10)/E10</f>
+        <v>32.7386850530898</v>
+      </c>
+      <c r="N22" s="6" t="n">
+        <f aca="false">100*ABS(E10-L22)/E10</f>
+        <v>5.66160074431671</v>
+      </c>
       <c r="O22" s="0" t="n">
         <v>1000</v>
       </c>
@@ -1100,7 +1266,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>6</v>
@@ -1114,8 +1280,11 @@
       <c r="E24" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F24" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="H24" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1157,7 +1326,12 @@
         <v>110.8762238471</v>
       </c>
       <c r="E25" s="2" t="n">
+        <f aca="false">I16/$I$8</f>
         <v>124.1813707088</v>
+      </c>
+      <c r="F25" s="0" t="n">
+        <f aca="false">J16/$I$8</f>
+        <v>153.984899678912</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>6</v>
@@ -1198,13 +1372,18 @@
         <v>552.2430126432</v>
       </c>
       <c r="E26" s="2" t="n">
+        <f aca="false">I17/$I$8</f>
         <v>618.5121741604</v>
+      </c>
+      <c r="F26" s="0" t="n">
+        <f aca="false">J17/$I$8</f>
+        <v>766.955095958896</v>
       </c>
       <c r="H26" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J26" s="2" t="s">
         <v>22</v>
@@ -1248,7 +1427,12 @@
         <v>1103.8621675961</v>
       </c>
       <c r="E27" s="2" t="n">
+        <f aca="false">I18/$I$8</f>
         <v>1236.3256277076</v>
+      </c>
+      <c r="F27" s="0" t="n">
+        <f aca="false">J18/$I$8</f>
+        <v>1533.04377835742</v>
       </c>
       <c r="H27" s="2" t="n">
         <v>1000</v>
@@ -1298,7 +1482,12 @@
         <v>2759.3925861018</v>
       </c>
       <c r="E28" s="2" t="n">
+        <f aca="false">I19/$I$8</f>
         <v>3090.519696434</v>
+      </c>
+      <c r="F28" s="0" t="n">
+        <f aca="false">J19/$I$8</f>
+        <v>3832.24442357816</v>
       </c>
       <c r="H28" s="2" t="n">
         <v>5000</v>
@@ -1348,7 +1537,12 @@
         <v>5519.3639080593</v>
       </c>
       <c r="E29" s="2" t="n">
+        <f aca="false">I20/$I$8</f>
         <v>6181.6875770264</v>
+      </c>
+      <c r="F29" s="0" t="n">
+        <f aca="false">J20/$I$8</f>
+        <v>7665.29259551274</v>
       </c>
       <c r="H29" s="2" t="n">
         <v>10000</v>
@@ -1380,7 +1574,12 @@
         <v>8277.2606269104</v>
       </c>
       <c r="E30" s="2" t="n">
+        <f aca="false">I21/$I$8</f>
         <v>9270.5319021396</v>
+      </c>
+      <c r="F30" s="0" t="n">
+        <f aca="false">J21/$I$8</f>
+        <v>11495.4595586531</v>
       </c>
       <c r="H30" s="2" t="n">
         <v>25000</v>
@@ -1412,7 +1611,12 @@
         <v>11037.7010080164</v>
       </c>
       <c r="E31" s="2" t="n">
+        <f aca="false">I22/$I$8</f>
         <v>12362.2251289784</v>
+      </c>
+      <c r="F31" s="0" t="n">
+        <f aca="false">J22/$I$8</f>
+        <v>15329.1591599332</v>
       </c>
       <c r="H31" s="2" t="n">
         <v>50000</v>
@@ -1469,7 +1673,7 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>6</v>
@@ -1483,8 +1687,11 @@
       <c r="E34" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="F34" s="0" t="s">
+        <v>26</v>
+      </c>
       <c r="H34" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I34" s="0" t="n">
         <v>2.73237373737374</v>
@@ -1515,8 +1722,12 @@
       <c r="E35" s="2" t="n">
         <v>100.470364651133</v>
       </c>
+      <c r="F35" s="0" t="n">
+        <f aca="false">J16/$J$8</f>
+        <v>124.583252167405</v>
+      </c>
       <c r="O35" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1535,6 +1746,10 @@
       <c r="E36" s="2" t="n">
         <v>500.414380388673</v>
       </c>
+      <c r="F36" s="0" t="n">
+        <f aca="false">J17/$J$8</f>
+        <v>620.513831681955</v>
+      </c>
       <c r="H36" s="2" t="s">
         <v>7</v>
       </c>
@@ -1564,11 +1779,15 @@
       <c r="E37" s="2" t="n">
         <v>1000.26345283786</v>
       </c>
+      <c r="F37" s="0" t="n">
+        <f aca="false">J18/$J$8</f>
+        <v>1240.32668151895</v>
+      </c>
       <c r="H37" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>22</v>
@@ -1614,6 +1833,10 @@
       <c r="E38" s="2" t="n">
         <v>2500.42046637055</v>
       </c>
+      <c r="F38" s="0" t="n">
+        <f aca="false">J19/$J$8</f>
+        <v>3100.52137829948</v>
+      </c>
       <c r="H38" s="2" t="n">
         <v>1000</v>
       </c>
@@ -1664,6 +1887,10 @@
       <c r="E39" s="2" t="n">
         <v>5001.36535358123</v>
       </c>
+      <c r="F39" s="0" t="n">
+        <f aca="false">J20/$J$8</f>
+        <v>6201.69303844073</v>
+      </c>
       <c r="H39" s="2" t="n">
         <v>5000</v>
       </c>
@@ -1714,6 +1941,10 @@
       <c r="E40" s="2" t="n">
         <v>7500.43034153689</v>
       </c>
+      <c r="F40" s="0" t="n">
+        <f aca="false">J21/$J$8</f>
+        <v>9300.53362350575</v>
+      </c>
       <c r="H40" s="2" t="n">
         <v>10000</v>
       </c>
@@ -1763,6 +1994,10 @@
       </c>
       <c r="E41" s="2" t="n">
         <v>10001.8002661638</v>
+      </c>
+      <c r="F41" s="0" t="n">
+        <f aca="false">J22/$J$8</f>
+        <v>12402.2323300431</v>
       </c>
       <c r="H41" s="2" t="n">
         <v>25000</v>
@@ -1881,13 +2116,13 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
@@ -1919,7 +2154,7 @@
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
       <c r="H45" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I45" s="0" t="n">
         <v>2.88788131313131</v>
@@ -2018,7 +2253,7 @@
         <v>5</v>
       </c>
       <c r="I48" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="J48" s="2" t="s">
         <v>22</v>
@@ -2233,7 +2468,7 @@
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="H53" s="2" t="n">
         <v>50000</v>
@@ -2271,7 +2506,7 @@
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>6</v>
@@ -2296,7 +2531,7 @@
         <v>0.0005035155</v>
       </c>
       <c r="O54" s="0" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2350,7 +2585,7 @@
       </c>
       <c r="E56" s="2"/>
       <c r="H56" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I56" s="0" t="n">
         <v>3.58892171717171</v>
@@ -2434,7 +2669,7 @@
       </c>
       <c r="E58" s="2"/>
       <c r="H58" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="I58" s="1"/>
       <c r="J58" s="1"/>
@@ -2518,7 +2753,7 @@
         <v>5</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J60" s="2" t="s">
         <v>22</v>
@@ -2650,7 +2885,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>6</v>
@@ -2661,7 +2896,9 @@
       <c r="D64" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E64" s="2"/>
+      <c r="E64" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H64" s="2" t="n">
         <v>25000</v>
       </c>
@@ -2675,7 +2912,7 @@
         <v>6408546627.93452</v>
       </c>
       <c r="O64" s="0" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2691,7 +2928,10 @@
       <c r="D65" s="2" t="n">
         <v>170.553770514852</v>
       </c>
-      <c r="E65" s="2"/>
+      <c r="E65" s="2" t="n">
+        <f aca="false">ABS(E25-E4)/E4*100</f>
+        <v>14.8762611003129</v>
+      </c>
       <c r="H65" s="2" t="n">
         <v>50000</v>
       </c>
@@ -2742,7 +2982,10 @@
       <c r="D66" s="2" t="n">
         <v>170.933022813904</v>
       </c>
-      <c r="E66" s="2"/>
+      <c r="E66" s="2" t="n">
+        <f aca="false">ABS(E26-E5)/E5*100</f>
+        <v>15.3095375115906</v>
+      </c>
       <c r="H66" s="2" t="n">
         <v>75000</v>
       </c>
@@ -2767,7 +3010,7 @@
       <c r="R66" s="3" t="n">
         <v>110.8762238471</v>
       </c>
-      <c r="S66" s="6" t="n">
+      <c r="S66" s="7" t="n">
         <v>124.1813707088</v>
       </c>
       <c r="T66" s="3" t="n">
@@ -2797,7 +3040,10 @@
       <c r="D67" s="2" t="n">
         <v>170.735264132191</v>
       </c>
-      <c r="E67" s="2"/>
+      <c r="E67" s="2" t="n">
+        <f aca="false">ABS(E27-E6)/E6*100</f>
+        <v>14.9470199737045</v>
+      </c>
       <c r="H67" s="2" t="n">
         <v>100000</v>
       </c>
@@ -2822,7 +3068,7 @@
       <c r="R67" s="3" t="n">
         <v>552.2430126432</v>
       </c>
-      <c r="S67" s="6" t="n">
+      <c r="S67" s="7" t="n">
         <v>618.5121741604</v>
       </c>
       <c r="T67" s="3" t="n">
@@ -2852,7 +3098,10 @@
       <c r="D68" s="2" t="n">
         <v>170.238842785146</v>
       </c>
-      <c r="E68" s="2"/>
+      <c r="E68" s="2" t="n">
+        <f aca="false">ABS(E28-E7)/E7*100</f>
+        <v>17.5790599242499</v>
+      </c>
       <c r="O68" s="2" t="n">
         <v>10000</v>
       </c>
@@ -2865,7 +3114,7 @@
       <c r="R68" s="3" t="n">
         <v>1103.8621675961</v>
       </c>
-      <c r="S68" s="6" t="n">
+      <c r="S68" s="7" t="n">
         <v>1236.3256277076</v>
       </c>
       <c r="T68" s="3" t="n">
@@ -2895,7 +3144,10 @@
       <c r="D69" s="2" t="n">
         <v>169.737953893087</v>
       </c>
-      <c r="E69" s="2"/>
+      <c r="E69" s="2" t="n">
+        <f aca="false">ABS(E29-E8)/E8*100</f>
+        <v>16.1311140454845</v>
+      </c>
       <c r="H69" s="2" t="s">
         <v>7</v>
       </c>
@@ -2911,7 +3163,7 @@
       <c r="R69" s="3" t="n">
         <v>2759.3925861018</v>
       </c>
-      <c r="S69" s="6" t="n">
+      <c r="S69" s="7" t="n">
         <v>3090.519696434</v>
       </c>
       <c r="T69" s="3" t="n">
@@ -2941,12 +3193,15 @@
       <c r="D70" s="2" t="n">
         <v>169.541965170294</v>
       </c>
-      <c r="E70" s="2"/>
+      <c r="E70" s="2" t="n">
+        <f aca="false">ABS(E30-E9)/E9*100</f>
+        <v>15.3483627638314</v>
+      </c>
       <c r="H70" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I70" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J70" s="2" t="s">
         <v>22</v>
@@ -2966,7 +3221,7 @@
       <c r="R70" s="3" t="n">
         <v>5519.3639080593</v>
       </c>
-      <c r="S70" s="6" t="n">
+      <c r="S70" s="7" t="n">
         <v>6181.6875770264</v>
       </c>
       <c r="T70" s="3" t="n">
@@ -2996,7 +3251,10 @@
       <c r="D71" s="2" t="n">
         <v>169.33984242865</v>
       </c>
-      <c r="E71" s="2"/>
+      <c r="E71" s="2" t="n">
+        <f aca="false">ABS(E31-E10)/E10*100</f>
+        <v>7.0473266557176</v>
+      </c>
       <c r="H71" s="2" t="n">
         <v>1000</v>
       </c>
@@ -3021,7 +3279,7 @@
       <c r="R71" s="3" t="n">
         <v>8277.2606269104</v>
       </c>
-      <c r="S71" s="6" t="n">
+      <c r="S71" s="7" t="n">
         <v>9270.5319021396</v>
       </c>
       <c r="T71" s="3" t="n">
@@ -3068,7 +3326,7 @@
       <c r="R72" s="3" t="n">
         <v>11037.7010080164</v>
       </c>
-      <c r="S72" s="6" t="n">
+      <c r="S72" s="7" t="n">
         <v>12362.2251289784</v>
       </c>
       <c r="T72" s="3" t="n">
@@ -3102,12 +3360,12 @@
         <v>2554699449.56524</v>
       </c>
       <c r="O73" s="0" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>6</v>
@@ -3118,7 +3376,9 @@
       <c r="D74" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E74" s="2"/>
+      <c r="E74" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="H74" s="2" t="n">
         <v>25000</v>
       </c>
@@ -3169,6 +3429,10 @@
       <c r="D75" s="0" t="n">
         <v>110.430710400467</v>
       </c>
+      <c r="E75" s="0" t="n">
+        <f aca="false">ABS(E35-E4)/E4*100</f>
+        <v>7.05804118097635</v>
+      </c>
       <c r="H75" s="2" t="n">
         <v>50000</v>
       </c>
@@ -3193,7 +3457,7 @@
       <c r="R75" s="3" t="n">
         <v>86.2370629922</v>
       </c>
-      <c r="S75" s="6" t="n">
+      <c r="S75" s="7" t="n">
         <v>100.470364651133</v>
       </c>
       <c r="T75" s="3" t="n">
@@ -3223,6 +3487,10 @@
       <c r="D76" s="0" t="n">
         <v>110.725684410798</v>
       </c>
+      <c r="E76" s="0" t="n">
+        <f aca="false">ABS(E36-E5)/E5*100</f>
+        <v>6.70749392266136</v>
+      </c>
       <c r="H76" s="2" t="n">
         <v>75000</v>
       </c>
@@ -3247,7 +3515,7 @@
       <c r="R76" s="3" t="n">
         <v>429.5223431669</v>
       </c>
-      <c r="S76" s="6" t="n">
+      <c r="S76" s="7" t="n">
         <v>500.414380388673</v>
       </c>
       <c r="T76" s="3" t="n">
@@ -3277,6 +3545,10 @@
       <c r="D77" s="0" t="n">
         <v>110.571872102801</v>
       </c>
+      <c r="E77" s="0" t="n">
+        <f aca="false">ABS(E37-E6)/E6*100</f>
+        <v>7.00079290153394</v>
+      </c>
       <c r="H77" s="2" t="n">
         <v>100000</v>
       </c>
@@ -3301,7 +3573,7 @@
       <c r="R77" s="3" t="n">
         <v>858.5594636858</v>
       </c>
-      <c r="S77" s="6" t="n">
+      <c r="S77" s="7" t="n">
         <v>1000.26345283786</v>
       </c>
       <c r="T77" s="3" t="n">
@@ -3331,6 +3603,10 @@
       <c r="D78" s="0" t="n">
         <v>110.185766610666</v>
       </c>
+      <c r="E78" s="0" t="n">
+        <f aca="false">ABS(E38-E7)/E7*100</f>
+        <v>4.87131074089813</v>
+      </c>
       <c r="O78" s="2" t="n">
         <v>25000</v>
       </c>
@@ -3343,7 +3619,7 @@
       <c r="R78" s="3" t="n">
         <v>2146.1942336347</v>
       </c>
-      <c r="S78" s="6" t="n">
+      <c r="S78" s="7" t="n">
         <v>2500.42046637055</v>
       </c>
       <c r="T78" s="3" t="n">
@@ -3373,6 +3649,10 @@
       <c r="D79" s="0" t="n">
         <v>109.796186361288</v>
       </c>
+      <c r="E79" s="0" t="n">
+        <f aca="false">ABS(E39-E8)/E8*100</f>
+        <v>6.0427879890902</v>
+      </c>
       <c r="H79" s="2" t="s">
         <v>8</v>
       </c>
@@ -3388,7 +3668,7 @@
       <c r="R79" s="3" t="n">
         <v>4292.8385951572</v>
       </c>
-      <c r="S79" s="6" t="n">
+      <c r="S79" s="7" t="n">
         <v>5001.36535358123</v>
       </c>
       <c r="T79" s="3" t="n">
@@ -3418,11 +3698,15 @@
       <c r="D80" s="0" t="n">
         <v>109.643750688005</v>
       </c>
+      <c r="E80" s="0" t="n">
+        <f aca="false">ABS(E40-E9)/E9*100</f>
+        <v>6.67608190628536</v>
+      </c>
       <c r="H80" s="2" t="s">
         <v>5</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>22</v>
@@ -3442,7 +3726,7 @@
       <c r="R80" s="3" t="n">
         <v>6437.8693764858</v>
       </c>
-      <c r="S80" s="6" t="n">
+      <c r="S80" s="7" t="n">
         <v>7500.43034153689</v>
       </c>
       <c r="T80" s="3" t="n">
@@ -3472,6 +3756,10 @@
       <c r="D81" s="0" t="n">
         <v>109.486544111174</v>
       </c>
+      <c r="E81" s="0" t="n">
+        <f aca="false">ABS(E41-E10)/E10*100</f>
+        <v>13.3921305374449</v>
+      </c>
       <c r="H81" s="2" t="n">
         <v>1000</v>
       </c>
@@ -3496,7 +3784,7 @@
       <c r="R81" s="3" t="n">
         <v>8584.8785617906</v>
       </c>
-      <c r="S81" s="6" t="n">
+      <c r="S81" s="7" t="n">
         <v>10001.8002661638</v>
       </c>
       <c r="T81" s="3" t="n">
@@ -3527,12 +3815,12 @@
         <v>524407386.305137</v>
       </c>
       <c r="O82" s="0" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="H83" s="2" t="n">
         <v>10000</v>
@@ -3567,7 +3855,7 @@
     </row>
     <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A84" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>6</v>
@@ -3875,7 +4163,7 @@
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B93" s="0" t="s">
         <v>6</v>
@@ -3885,6 +4173,18 @@
       </c>
       <c r="D93" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="O93" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="T93" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="X93" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB93" s="0" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3900,6 +4200,54 @@
       <c r="D94" s="0" t="n">
         <v>169.3398424287</v>
       </c>
+      <c r="P94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q94" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="R94" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="S94" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="T94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="U94" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="V94" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="W94" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="X94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y94" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z94" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="AA94" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="AB94" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="AC94" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="AD94" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE94" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="0" t="s">
@@ -3914,10 +4262,69 @@
       <c r="D95" s="0" t="n">
         <v>109.4865441112</v>
       </c>
+      <c r="O95" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="P95" s="0" t="n">
+        <v>127.260545824744</v>
+      </c>
+      <c r="Q95" s="0" t="n">
+        <v>123.681170335407</v>
+      </c>
+      <c r="R95" s="0" t="n">
+        <v>111.103982187839</v>
+      </c>
+      <c r="S95" s="0" t="n">
+        <v>15.4759752256318</v>
+      </c>
+      <c r="T95" s="0" t="n">
+        <v>122.775283603106</v>
+      </c>
+      <c r="U95" s="0" t="n">
+        <v>123.649914476707</v>
+      </c>
+      <c r="V95" s="0" t="n">
+        <v>111.078977869837</v>
+      </c>
+      <c r="W95" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="X95" s="0" t="n">
+        <f aca="false">ABS(P95-T95)/P95*100</f>
+        <v>3.52447193477738</v>
+      </c>
+      <c r="Y95" s="0" t="n">
+        <f aca="false">ABS(Q95-U95)/Q95*100</f>
+        <v>0.0252713154435056</v>
+      </c>
+      <c r="Z95" s="0" t="n">
+        <f aca="false">ABS(R95-V95)/R95*100</f>
+        <v>0.0225053301503542</v>
+      </c>
+      <c r="AA95" s="0" t="n">
+        <f aca="false">ABS(S95-W95)</f>
+        <v>0.524024774368201</v>
+      </c>
+      <c r="AB95" s="0" t="n">
+        <f aca="false">X95/T95*100</f>
+        <v>2.87066894194347</v>
+      </c>
+      <c r="AC95" s="0" t="n">
+        <f aca="false">Y95/U95*100</f>
+        <v>0.0204377945188682</v>
+      </c>
+      <c r="AD95" s="0" t="n">
+        <f aca="false">Z95/V95*100</f>
+        <v>0.0202606565003921</v>
+      </c>
+      <c r="AE95" s="0" t="n">
+        <f aca="false">AA95/W95*100</f>
+        <v>3.27515483980125</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B96" s="0" t="n">
         <v>126.2030377604</v>
@@ -3928,24 +4335,266 @@
       <c r="D96" s="0" t="n">
         <v>110.1319029162</v>
       </c>
+      <c r="O96" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="P96" s="0" t="n">
+        <v>127.022930843836</v>
+      </c>
+      <c r="Q96" s="0" t="n">
+        <v>124.060027127379</v>
+      </c>
+      <c r="R96" s="0" t="n">
+        <v>111.27226752587</v>
+      </c>
+      <c r="S96" s="0" t="n">
+        <v>10.8484139473245</v>
+      </c>
+      <c r="T96" s="0" t="n">
+        <v>123.47146839539</v>
+      </c>
+      <c r="U96" s="0" t="n">
+        <v>124.178344086502</v>
+      </c>
+      <c r="V96" s="0" t="n">
+        <v>111.374860597537</v>
+      </c>
+      <c r="W96" s="8" t="n">
+        <f aca="false">ABS((I17/2930145161.3)-E5)/E5*100</f>
+        <v>1.61789675598196</v>
+      </c>
+      <c r="X96" s="0" t="n">
+        <f aca="false">ABS(P96-T96)/P96*100</f>
+        <v>2.79592229911041</v>
+      </c>
+      <c r="Y96" s="0" t="n">
+        <f aca="false">ABS(Q96-U96)/Q96*100</f>
+        <v>0.0953707345245265</v>
+      </c>
+      <c r="Z96" s="0" t="n">
+        <f aca="false">ABS(R96-V96)/R96*100</f>
+        <v>0.0922000368538943</v>
+      </c>
+      <c r="AA96" s="0" t="n">
+        <f aca="false">ABS(S96-W96)</f>
+        <v>9.23051719134254</v>
+      </c>
+      <c r="AB96" s="0" t="n">
+        <f aca="false">X96/T96*100</f>
+        <v>2.26442783539035</v>
+      </c>
+      <c r="AC96" s="0" t="n">
+        <f aca="false">Y96/U96*100</f>
+        <v>0.0768014223624143</v>
+      </c>
+      <c r="AD96" s="0" t="n">
+        <f aca="false">Z96/V96*100</f>
+        <v>0.0827835261559315</v>
+      </c>
+      <c r="AE96" s="0" t="n">
+        <f aca="false">AA96/W96*100</f>
+        <v>570.525724661597</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O97" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P97" s="0" t="n">
+        <v>126.313622143246</v>
+      </c>
+      <c r="Q97" s="0" t="n">
+        <v>123.629943799774</v>
+      </c>
+      <c r="R97" s="0" t="n">
+        <v>111.092924807485</v>
+      </c>
+      <c r="S97" s="0" t="n">
+        <v>21.4762408123745</v>
+      </c>
+      <c r="T97" s="0" t="n">
+        <v>122.794642425541</v>
+      </c>
+      <c r="U97" s="0" t="n">
+        <v>123.768059682806</v>
+      </c>
+      <c r="V97" s="0" t="n">
+        <v>111.220574444658</v>
+      </c>
+      <c r="W97" s="8" t="n">
+        <f aca="false">ABS((I18/2930145161.3)-E6)/E6*100</f>
+        <v>1.92719673766381</v>
+      </c>
+      <c r="X97" s="0" t="n">
+        <f aca="false">ABS(P97-T97)/P97*100</f>
+        <v>2.78590674386167</v>
+      </c>
+      <c r="Y97" s="0" t="n">
+        <f aca="false">ABS(Q97-U97)/Q97*100</f>
+        <v>0.111717176913189</v>
+      </c>
+      <c r="Z97" s="0" t="n">
+        <f aca="false">ABS(R97-V97)/R97*100</f>
+        <v>0.114903480481576</v>
+      </c>
+      <c r="AA97" s="0" t="n">
+        <f aca="false">ABS(S97-W97)</f>
+        <v>19.5490440747107</v>
+      </c>
+      <c r="AB97" s="0" t="n">
+        <f aca="false">X97/T97*100</f>
+        <v>2.26875268239081</v>
+      </c>
+      <c r="AC97" s="0" t="n">
+        <f aca="false">Y97/U97*100</f>
+        <v>0.0902633338516406</v>
+      </c>
+      <c r="AD97" s="0" t="n">
+        <f aca="false">Z97/V97*100</f>
+        <v>0.1033113531874</v>
+      </c>
+      <c r="AE97" s="0" t="n">
+        <f aca="false">AA97/W97*100</f>
+        <v>1014.37718799838</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B98" s="8"/>
-      <c r="C98" s="8"/>
-      <c r="D98" s="8"/>
-      <c r="E98" s="8"/>
+      <c r="A98" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B98" s="10"/>
+      <c r="C98" s="10"/>
+      <c r="D98" s="10"/>
+      <c r="E98" s="10"/>
+      <c r="O98" s="0" t="n">
+        <v>25000</v>
+      </c>
+      <c r="P98" s="0" t="n">
+        <v>125.949978007765</v>
+      </c>
+      <c r="Q98" s="0" t="n">
+        <v>123.632890310969</v>
+      </c>
+      <c r="R98" s="0" t="n">
+        <v>110.685813688158</v>
+      </c>
+      <c r="S98" s="0" t="n">
+        <v>22.397002038486</v>
+      </c>
+      <c r="T98" s="0" t="n">
+        <v>123.473953949445</v>
+      </c>
+      <c r="U98" s="0" t="n">
+        <v>123.800220846314</v>
+      </c>
+      <c r="V98" s="0" t="n">
+        <v>110.833279489098</v>
+      </c>
+      <c r="W98" s="8" t="n">
+        <f aca="false">ABS((I19/2930145161.3)-E7)/E7*100</f>
+        <v>0.31845988142472</v>
+      </c>
+      <c r="X98" s="0" t="n">
+        <f aca="false">ABS(P98-T98)/P98*100</f>
+        <v>1.96587891279138</v>
+      </c>
+      <c r="Y98" s="0" t="n">
+        <f aca="false">ABS(Q98-U98)/Q98*100</f>
+        <v>0.135344676424354</v>
+      </c>
+      <c r="Z98" s="0" t="n">
+        <f aca="false">ABS(R98-V98)/R98*100</f>
+        <v>0.133229179085048</v>
+      </c>
+      <c r="AA98" s="0" t="n">
+        <f aca="false">ABS(S98-W98)</f>
+        <v>22.0785421570613</v>
+      </c>
+      <c r="AB98" s="0" t="n">
+        <f aca="false">X98/T98*100</f>
+        <v>1.59214056884927</v>
+      </c>
+      <c r="AC98" s="0" t="n">
+        <f aca="false">Y98/U98*100</f>
+        <v>0.109325068646179</v>
+      </c>
+      <c r="AD98" s="0" t="n">
+        <f aca="false">Z98/V98*100</f>
+        <v>0.12020683651985</v>
+      </c>
+      <c r="AE98" s="0" t="n">
+        <f aca="false">AA98/W98*100</f>
+        <v>6932.91163027717</v>
+      </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="O99" s="0" t="n">
+        <v>50000</v>
+      </c>
+      <c r="P99" s="0" t="n">
+        <v>125.352281689144</v>
+      </c>
+      <c r="Q99" s="0" t="n">
+        <v>122.696669341942</v>
+      </c>
+      <c r="R99" s="0" t="n">
+        <v>110.281556788388</v>
+      </c>
+      <c r="S99" s="0" t="n">
+        <v>16.6131052423114</v>
+      </c>
+      <c r="T99" s="0" t="n">
+        <v>123.9740098939</v>
+      </c>
+      <c r="U99" s="0" t="n">
+        <v>122.825372532345</v>
+      </c>
+      <c r="V99" s="0" t="n">
+        <v>110.442499071735</v>
+      </c>
+      <c r="W99" s="8" t="n">
+        <f aca="false">ABS((I20/2930145161.3)-E8)/E8*100</f>
+        <v>0.916927615660088</v>
+      </c>
+      <c r="X99" s="0" t="n">
+        <f aca="false">ABS(P99-T99)/P99*100</f>
+        <v>1.09951871371722</v>
+      </c>
+      <c r="Y99" s="0" t="n">
+        <f aca="false">ABS(Q99-U99)/Q99*100</f>
+        <v>0.104895423073249</v>
+      </c>
+      <c r="Z99" s="0" t="n">
+        <f aca="false">ABS(R99-V99)/R99*100</f>
+        <v>0.14593762369131</v>
+      </c>
+      <c r="AA99" s="0" t="n">
+        <f aca="false">ABS(S99-W99)</f>
+        <v>15.6961776266513</v>
+      </c>
+      <c r="AB99" s="0" t="n">
+        <f aca="false">X99/T99*100</f>
+        <v>0.886894531086165</v>
+      </c>
+      <c r="AC99" s="0" t="n">
+        <f aca="false">Y99/U99*100</f>
+        <v>0.0854020801326092</v>
+      </c>
+      <c r="AD99" s="0" t="n">
+        <f aca="false">Z99/V99*100</f>
+        <v>0.132139008912249</v>
+      </c>
+      <c r="AE99" s="0" t="n">
+        <f aca="false">AA99/W99*100</f>
+        <v>1711.82297910744</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B100" s="0" t="s">
         <v>6</v>
@@ -3955,6 +4604,66 @@
       </c>
       <c r="D100" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="O100" s="0" t="n">
+        <v>75000</v>
+      </c>
+      <c r="P100" s="0" t="n">
+        <v>125.153987580039</v>
+      </c>
+      <c r="Q100" s="0" t="n">
+        <v>122.659192506874</v>
+      </c>
+      <c r="R100" s="0" t="n">
+        <v>110.120194786699</v>
+      </c>
+      <c r="S100" s="0" t="n">
+        <v>35.58727152408</v>
+      </c>
+      <c r="T100" s="0" t="n">
+        <v>126.390472993283</v>
+      </c>
+      <c r="U100" s="0" t="n">
+        <v>122.854178384527</v>
+      </c>
+      <c r="V100" s="0" t="n">
+        <v>110.28959379452</v>
+      </c>
+      <c r="W100" s="8" t="n">
+        <f aca="false">ABS((I21/2930145161.3)-E9)/E9*100</f>
+        <v>1.5847710488041</v>
+      </c>
+      <c r="X100" s="0" t="n">
+        <f aca="false">ABS(P100-T100)/P100*100</f>
+        <v>0.987971248182285</v>
+      </c>
+      <c r="Y100" s="0" t="n">
+        <f aca="false">ABS(Q100-U100)/Q100*100</f>
+        <v>0.158965564396673</v>
+      </c>
+      <c r="Z100" s="0" t="n">
+        <f aca="false">ABS(R100-V100)/R100*100</f>
+        <v>0.15383100996942</v>
+      </c>
+      <c r="AA100" s="0" t="n">
+        <f aca="false">ABS(S100-W100)</f>
+        <v>34.0025004752759</v>
+      </c>
+      <c r="AB100" s="0" t="n">
+        <f aca="false">X100/T100*100</f>
+        <v>0.78168173975802</v>
+      </c>
+      <c r="AC100" s="0" t="n">
+        <f aca="false">Y100/U100*100</f>
+        <v>0.129393697867662</v>
+      </c>
+      <c r="AD100" s="0" t="n">
+        <f aca="false">Z100/V100*100</f>
+        <v>0.139479169953261</v>
+      </c>
+      <c r="AE100" s="0" t="n">
+        <f aca="false">AA100/W100*100</f>
+        <v>2145.57809476232</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3970,6 +4679,66 @@
       <c r="D101" s="0" t="n">
         <v>54.1080577827666</v>
       </c>
+      <c r="O101" s="0" t="n">
+        <v>100000</v>
+      </c>
+      <c r="P101" s="0" t="n">
+        <v>125.085796471176</v>
+      </c>
+      <c r="Q101" s="0" t="n">
+        <v>122.413330207488</v>
+      </c>
+      <c r="R101" s="0" t="n">
+        <v>109.955115526649</v>
+      </c>
+      <c r="S101" s="0" t="n">
+        <v>18.2845976379756</v>
+      </c>
+      <c r="T101" s="0" t="n">
+        <v>126.203037760438</v>
+      </c>
+      <c r="U101" s="0" t="n">
+        <v>122.611360877376</v>
+      </c>
+      <c r="V101" s="0" t="n">
+        <v>110.131902916184</v>
+      </c>
+      <c r="W101" s="8" t="n">
+        <f aca="false">ABS((I22/2930145161.3)-E10)/E10*100</f>
+        <v>8.6672154766007</v>
+      </c>
+      <c r="X101" s="0" t="n">
+        <f aca="false">ABS(P101-T101)/P101*100</f>
+        <v>0.893179977887661</v>
+      </c>
+      <c r="Y101" s="0" t="n">
+        <f aca="false">ABS(Q101-U101)/Q101*100</f>
+        <v>0.161772144873647</v>
+      </c>
+      <c r="Z101" s="0" t="n">
+        <f aca="false">ABS(R101-V101)/R101*100</f>
+        <v>0.160781414023503</v>
+      </c>
+      <c r="AA101" s="0" t="n">
+        <f aca="false">ABS(S101-W101)</f>
+        <v>9.6173821613749</v>
+      </c>
+      <c r="AB101" s="0" t="n">
+        <f aca="false">X101/T101*100</f>
+        <v>0.707732550450267</v>
+      </c>
+      <c r="AC101" s="0" t="n">
+        <f aca="false">Y101/U101*100</f>
+        <v>0.131938952243941</v>
+      </c>
+      <c r="AD101" s="0" t="n">
+        <f aca="false">Z101/V101*100</f>
+        <v>0.14598986285188</v>
+      </c>
+      <c r="AE101" s="0" t="n">
+        <f aca="false">AA101/W101*100</f>
+        <v>110.962767538657</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="0" t="n">
@@ -4040,6 +4809,9 @@
       <c r="D106" s="0" t="n">
         <v>4058.48286545563</v>
       </c>
+      <c r="O106" s="0" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A107" s="0" t="n">
@@ -4054,15 +4826,68 @@
       <c r="D107" s="0" t="n">
         <v>5415.97654358062</v>
       </c>
+      <c r="P107" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q107" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R107" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S107" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T107" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O108" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="P108" s="3" t="n">
+        <v>134.9797507704</v>
+      </c>
+      <c r="Q108" s="3" t="n">
+        <v>124.1813707088</v>
+      </c>
+      <c r="R108" s="3" t="n">
+        <v>110.8762238471</v>
+      </c>
+      <c r="S108" s="7" t="n">
+        <v>124.1813707088</v>
+      </c>
+      <c r="T108" s="0" t="n">
+        <v>153.984899678912</v>
+      </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A109" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="O109" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="P109" s="3" t="n">
+        <v>672.2958414787</v>
+      </c>
+      <c r="Q109" s="3" t="n">
+        <v>618.5121741604</v>
+      </c>
+      <c r="R109" s="3" t="n">
+        <v>552.2430126432</v>
+      </c>
+      <c r="S109" s="7" t="n">
+        <v>618.5121741604</v>
+      </c>
+      <c r="T109" s="0" t="n">
+        <v>766.955095958896</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A110" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B110" s="0" t="s">
         <v>6</v>
@@ -4072,6 +4897,24 @@
       </c>
       <c r="D110" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="O110" s="2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P110" s="3" t="n">
+        <v>1343.83220403</v>
+      </c>
+      <c r="Q110" s="3" t="n">
+        <v>1236.3256277076</v>
+      </c>
+      <c r="R110" s="3" t="n">
+        <v>1103.8621675961</v>
+      </c>
+      <c r="S110" s="7" t="n">
+        <v>1236.3256277076</v>
+      </c>
+      <c r="T110" s="0" t="n">
+        <v>1533.04377835742</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4087,6 +4930,24 @@
       <c r="D111" s="0" t="n">
         <v>42.0840449421518</v>
       </c>
+      <c r="O111" s="2" t="n">
+        <v>25000</v>
+      </c>
+      <c r="P111" s="3" t="n">
+        <v>3359.2605396022</v>
+      </c>
+      <c r="Q111" s="3" t="n">
+        <v>3090.519696434</v>
+      </c>
+      <c r="R111" s="3" t="n">
+        <v>2759.3925861018</v>
+      </c>
+      <c r="S111" s="7" t="n">
+        <v>3090.519696434</v>
+      </c>
+      <c r="T111" s="0" t="n">
+        <v>3832.24442357816</v>
+      </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="0" t="n">
@@ -4101,6 +4962,24 @@
       <c r="D112" s="0" t="n">
         <v>209.557694445777</v>
       </c>
+      <c r="O112" s="2" t="n">
+        <v>50000</v>
+      </c>
+      <c r="P112" s="3" t="n">
+        <v>6719.2256272026</v>
+      </c>
+      <c r="Q112" s="3" t="n">
+        <v>6181.6875770264</v>
+      </c>
+      <c r="R112" s="3" t="n">
+        <v>5519.3639080593</v>
+      </c>
+      <c r="S112" s="7" t="n">
+        <v>6181.6875770264</v>
+      </c>
+      <c r="T112" s="0" t="n">
+        <v>7665.29259551274</v>
+      </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="0" t="n">
@@ -4115,6 +4994,24 @@
       <c r="D113" s="0" t="n">
         <v>418.94666074288</v>
       </c>
+      <c r="O113" s="2" t="n">
+        <v>75000</v>
+      </c>
+      <c r="P113" s="3" t="n">
+        <v>10076.6651110213</v>
+      </c>
+      <c r="Q113" s="3" t="n">
+        <v>9270.5319021396</v>
+      </c>
+      <c r="R113" s="3" t="n">
+        <v>8277.2606269104</v>
+      </c>
+      <c r="S113" s="7" t="n">
+        <v>9270.5319021396</v>
+      </c>
+      <c r="T113" s="0" t="n">
+        <v>11495.4595586531</v>
+      </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="0" t="n">
@@ -4129,6 +5026,24 @@
       <c r="D114" s="0" t="n">
         <v>1048.5523756728</v>
       </c>
+      <c r="O114" s="2" t="n">
+        <v>100000</v>
+      </c>
+      <c r="P114" s="3" t="n">
+        <v>13437.2012271504</v>
+      </c>
+      <c r="Q114" s="3" t="n">
+        <v>12362.2251289784</v>
+      </c>
+      <c r="R114" s="3" t="n">
+        <v>11037.7010080164</v>
+      </c>
+      <c r="S114" s="7" t="n">
+        <v>12362.2251289784</v>
+      </c>
+      <c r="T114" s="0" t="n">
+        <v>15329.1591599332</v>
+      </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="0" t="n">
@@ -4157,6 +5072,9 @@
       <c r="D116" s="0" t="n">
         <v>3156.59778424327</v>
       </c>
+      <c r="O116" s="0" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="0" t="n">
@@ -4171,15 +5089,68 @@
       <c r="D117" s="0" t="n">
         <v>4212.4262005627</v>
       </c>
+      <c r="P117" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q117" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R117" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S117" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T117" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O118" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="P118" s="2" t="n">
+        <v>50.961647322</v>
+      </c>
+      <c r="Q118" s="2" t="n">
+        <v>48.0670908734</v>
+      </c>
+      <c r="R118" s="2" t="n">
+        <v>40.9812155403</v>
+      </c>
+      <c r="S118" s="3" t="n">
+        <v>108.100115306122</v>
+      </c>
+      <c r="T118" s="3" t="n">
+        <v>108.100115306122</v>
+      </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
+      </c>
+      <c r="O119" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="P119" s="2" t="n">
+        <v>253.0347589385</v>
+      </c>
+      <c r="Q119" s="2" t="n">
+        <v>238.844211824</v>
+      </c>
+      <c r="R119" s="2" t="n">
+        <v>203.8300857192</v>
+      </c>
+      <c r="S119" s="3" t="n">
+        <v>536.392901669759</v>
+      </c>
+      <c r="T119" s="3" t="n">
+        <v>536.392901669759</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B120" s="0" t="s">
         <v>6</v>
@@ -4189,6 +5160,24 @@
       </c>
       <c r="D120" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="O120" s="2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P120" s="2" t="n">
+        <v>507.3201856153</v>
+      </c>
+      <c r="Q120" s="2" t="n">
+        <v>478.2939653073</v>
+      </c>
+      <c r="R120" s="2" t="n">
+        <v>407.727516079</v>
+      </c>
+      <c r="S120" s="3" t="n">
+        <v>1075.56126987061</v>
+      </c>
+      <c r="T120" s="3" t="n">
+        <v>1075.56126987061</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4204,6 +5193,24 @@
       <c r="D121" s="0" t="n">
         <v>42.2136919754211</v>
       </c>
+      <c r="O121" s="2" t="n">
+        <v>25000</v>
+      </c>
+      <c r="P121" s="2" t="n">
+        <v>1264.3246831347</v>
+      </c>
+      <c r="Q121" s="2" t="n">
+        <v>1195.4492135747</v>
+      </c>
+      <c r="R121" s="2" t="n">
+        <v>1021.0939913977</v>
+      </c>
+      <c r="S121" s="3" t="n">
+        <v>2628.46096781609</v>
+      </c>
+      <c r="T121" s="3" t="n">
+        <v>2628.46096781609</v>
+      </c>
     </row>
     <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="0" t="n">
@@ -4218,6 +5225,24 @@
       <c r="D122" s="0" t="n">
         <v>210.203272441452</v>
       </c>
+      <c r="O122" s="2" t="n">
+        <v>50000</v>
+      </c>
+      <c r="P122" s="2" t="n">
+        <v>2523.2683517233</v>
+      </c>
+      <c r="Q122" s="2" t="n">
+        <v>2401.6102937286</v>
+      </c>
+      <c r="R122" s="2" t="n">
+        <v>2046.1947710358</v>
+      </c>
+      <c r="S122" s="3" t="n">
+        <v>5323.02443478261</v>
+      </c>
+      <c r="T122" s="3" t="n">
+        <v>5323.02443478261</v>
+      </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="0" t="n">
@@ -4232,6 +5257,24 @@
       <c r="D123" s="0" t="n">
         <v>420.23729693857</v>
       </c>
+      <c r="O123" s="2" t="n">
+        <v>75000</v>
+      </c>
+      <c r="P123" s="2" t="n">
+        <v>3743.6955213908</v>
+      </c>
+      <c r="Q123" s="2" t="n">
+        <v>3601.1730977794</v>
+      </c>
+      <c r="R123" s="2" t="n">
+        <v>3070.8615712885</v>
+      </c>
+      <c r="S123" s="3" t="n">
+        <v>8036.98611754069</v>
+      </c>
+      <c r="T123" s="3" t="n">
+        <v>8036.98611754069</v>
+      </c>
     </row>
     <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="0" t="n">
@@ -4246,6 +5289,24 @@
       <c r="D124" s="0" t="n">
         <v>1051.78261898521</v>
       </c>
+      <c r="O124" s="2" t="n">
+        <v>100000</v>
+      </c>
+      <c r="P124" s="2" t="n">
+        <v>4996.342818147</v>
+      </c>
+      <c r="Q124" s="2" t="n">
+        <v>4807.3910358311</v>
+      </c>
+      <c r="R124" s="2" t="n">
+        <v>4098.0572753325</v>
+      </c>
+      <c r="S124" s="3" t="n">
+        <v>11548.3735233645</v>
+      </c>
+      <c r="T124" s="3" t="n">
+        <v>11548.3735233645</v>
+      </c>
     </row>
     <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="0" t="n">
@@ -4288,10 +5349,30 @@
       <c r="D127" s="0" t="n">
         <v>4225.40329343768</v>
       </c>
+      <c r="O127" s="0" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P128" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q128" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R128" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="S128" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T128" s="0" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B129" s="0" t="s">
         <v>6</v>
@@ -4301,6 +5382,29 @@
       </c>
       <c r="D129" s="0" t="s">
         <v>8</v>
+      </c>
+      <c r="O129" s="2" t="n">
+        <v>1000</v>
+      </c>
+      <c r="P129" s="0" t="n">
+        <f aca="false">(P108-P118)/P118</f>
+        <v>1.64865360253238</v>
+      </c>
+      <c r="Q129" s="0" t="n">
+        <f aca="false">(Q108-Q118)/Q118</f>
+        <v>1.58350086207362</v>
+      </c>
+      <c r="R129" s="0" t="n">
+        <f aca="false">(R108-R118)/R118</f>
+        <v>1.70553770514852</v>
+      </c>
+      <c r="S129" s="0" t="n">
+        <f aca="false">(S108-S118)/S118</f>
+        <v>0.148762611003129</v>
+      </c>
+      <c r="T129" s="0" t="n">
+        <f aca="false">(T108-T118)/T118</f>
+        <v>0.42446563764388</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4316,6 +5420,29 @@
       <c r="D130" s="0" t="n">
         <v>32.1596107546151</v>
       </c>
+      <c r="O130" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="P130" s="0" t="n">
+        <f aca="false">(P109-P119)/P119</f>
+        <v>1.65693078808237</v>
+      </c>
+      <c r="Q130" s="0" t="n">
+        <f aca="false">(Q109-Q119)/Q119</f>
+        <v>1.58960503768109</v>
+      </c>
+      <c r="R130" s="0" t="n">
+        <f aca="false">(R109-R119)/R119</f>
+        <v>1.70933022813904</v>
+      </c>
+      <c r="S130" s="0" t="n">
+        <f aca="false">(S109-S119)/S119</f>
+        <v>0.153095375115906</v>
+      </c>
+      <c r="T130" s="0" t="n">
+        <f aca="false">(T109-T119)/T119</f>
+        <v>0.429838265143723</v>
+      </c>
     </row>
     <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="0" t="s">
@@ -4330,10 +5457,33 @@
       <c r="D131" s="0" t="n">
         <v>2.79080836470067</v>
       </c>
+      <c r="O131" s="2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="P131" s="0" t="n">
+        <f aca="false">(P110-P120)/P120</f>
+        <v>1.64888376637358</v>
+      </c>
+      <c r="Q131" s="0" t="n">
+        <f aca="false">(Q110-Q120)/Q120</f>
+        <v>1.5848656211108</v>
+      </c>
+      <c r="R131" s="0" t="n">
+        <f aca="false">(R110-R120)/R120</f>
+        <v>1.70735264132191</v>
+      </c>
+      <c r="S131" s="0" t="n">
+        <f aca="false">(S110-S120)/S120</f>
+        <v>0.149470199737045</v>
+      </c>
+      <c r="T131" s="0" t="n">
+        <f aca="false">(T110-T120)/T120</f>
+        <v>0.425343047673932</v>
+      </c>
     </row>
     <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="0" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B132" s="0" t="n">
         <v>0.243953606505694</v>
@@ -4344,19 +5494,113 @@
       <c r="D132" s="0" t="n">
         <v>3.10747287188282</v>
       </c>
+      <c r="O132" s="2" t="n">
+        <v>25000</v>
+      </c>
+      <c r="P132" s="0" t="n">
+        <f aca="false">(P111-P121)/P121</f>
+        <v>1.65696033970754</v>
+      </c>
+      <c r="Q132" s="0" t="n">
+        <f aca="false">(Q111-Q121)/Q121</f>
+        <v>1.58523713206733</v>
+      </c>
+      <c r="R132" s="0" t="n">
+        <f aca="false">(R111-R121)/R121</f>
+        <v>1.70238842785146</v>
+      </c>
+      <c r="S132" s="0" t="n">
+        <f aca="false">(S111-S121)/S121</f>
+        <v>0.175790599242499</v>
+      </c>
+      <c r="T132" s="0" t="n">
+        <f aca="false">(T111-T121)/T121</f>
+        <v>0.457980343060699</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O133" s="2" t="n">
+        <v>50000</v>
+      </c>
+      <c r="P133" s="0" t="n">
+        <f aca="false">(P112-P122)/P122</f>
+        <v>1.6629056804892</v>
+      </c>
+      <c r="Q133" s="0" t="n">
+        <f aca="false">(Q112-Q122)/Q122</f>
+        <v>1.57397613308405</v>
+      </c>
+      <c r="R133" s="0" t="n">
+        <f aca="false">(R112-R122)/R122</f>
+        <v>1.69737953893087</v>
+      </c>
+      <c r="S133" s="0" t="n">
+        <f aca="false">(S112-S122)/S122</f>
+        <v>0.161311140454845</v>
+      </c>
+      <c r="T133" s="0" t="n">
+        <f aca="false">(T112-T122)/T122</f>
+        <v>0.440025814164009</v>
+      </c>
     </row>
     <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
+      <c r="O134" s="2" t="n">
+        <v>75000</v>
+      </c>
+      <c r="P134" s="0" t="n">
+        <f aca="false">(P113-P123)/P123</f>
+        <v>1.69163585912504</v>
+      </c>
+      <c r="Q134" s="0" t="n">
+        <f aca="false">(Q113-Q123)/Q123</f>
+        <v>1.57430888502863</v>
+      </c>
+      <c r="R134" s="0" t="n">
+        <f aca="false">(R113-R123)/R123</f>
+        <v>1.69541965170294</v>
+      </c>
+      <c r="S134" s="0" t="n">
+        <f aca="false">(S113-S123)/S123</f>
+        <v>0.153483627638314</v>
+      </c>
+      <c r="T134" s="0" t="n">
+        <f aca="false">(T113-T123)/T123</f>
+        <v>0.430319698271508</v>
+      </c>
     </row>
     <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="0" t="s">
-        <v>45</v>
+        <v>53</v>
+      </c>
+      <c r="O135" s="2" t="n">
+        <v>100000</v>
+      </c>
+      <c r="P135" s="0" t="n">
+        <f aca="false">(P114-P124)/P124</f>
+        <v>1.6894073758001</v>
+      </c>
+      <c r="Q135" s="0" t="n">
+        <f aca="false">(Q114-Q124)/Q124</f>
+        <v>1.57150396895917</v>
+      </c>
+      <c r="R135" s="0" t="n">
+        <f aca="false">(R114-R124)/R124</f>
+        <v>1.6933984242865</v>
+      </c>
+      <c r="S135" s="0" t="n">
+        <f aca="false">(S114-S124)/S124</f>
+        <v>0.070473266557176</v>
+      </c>
+      <c r="T135" s="0" t="n">
+        <f aca="false">(T114-T124)/T124</f>
+        <v>0.327386850530897</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4389,7 +5633,7 @@
     </row>
     <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B140" s="0" t="s">
         <v>9</v>
@@ -4397,7 +5641,7 @@
     </row>
     <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A141" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B141" s="0" t="n">
         <v>12362.2251289784</v>
@@ -4405,7 +5649,7 @@
     </row>
     <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A142" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B142" s="0" t="n">
         <v>10001.8002661638</v>
@@ -4413,7 +5657,7 @@
     </row>
     <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A143" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B143" s="0" t="n">
         <v>17169.7571235811</v>
@@ -4421,7 +5665,7 @@
     </row>
     <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A144" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B144" s="0" t="n">
         <v>7726.3907056115</v>
@@ -4429,7 +5673,7 @@
     </row>
     <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A146" s="0" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B146" s="0" t="s">
         <v>9</v>
@@ -4437,7 +5681,7 @@
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A147" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="B147" s="0" t="n">
         <v>8.6215072033</v>
@@ -4445,7 +5689,7 @@
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A148" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="B148" s="0" t="n">
         <v>12.1185216802</v>
@@ -4453,7 +5697,7 @@
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A149" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="B149" s="0" t="n">
         <v>50.863204449</v>
@@ -4461,7 +5705,7 @@
     </row>
     <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A150" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="B150" s="0" t="n">
         <v>32.111557998</v>

</xml_diff>